<commit_message>
update to spreadsheet and pre-writing notes
</commit_message>
<xml_diff>
--- a/literature/Selling WSN.xlsx
+++ b/literature/Selling WSN.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="294">
   <si>
     <t>Micro-finance</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Coleman et al</t>
   </si>
   <si>
-    <t>Banjerjee et al</t>
-  </si>
-  <si>
     <t>Carrell &amp; Hoekstra</t>
   </si>
   <si>
@@ -81,33 +78,21 @@
     <t>Shue</t>
   </si>
   <si>
-    <t>Bertrand et al</t>
-  </si>
-  <si>
     <t>Kling</t>
   </si>
   <si>
     <t>Boboni and Finan</t>
   </si>
   <si>
-    <t>Dahl et al</t>
-  </si>
-  <si>
     <t>Grinblatt</t>
   </si>
   <si>
     <t>Kuhn</t>
   </si>
   <si>
-    <t>Guryan et al.</t>
-  </si>
-  <si>
     <t>Mas and Moretti</t>
   </si>
   <si>
-    <t>Bandiera et al.</t>
-  </si>
-  <si>
     <t>Manski</t>
   </si>
   <si>
@@ -174,9 +159,6 @@
     <t>Edin, Fredriksson, and Ashlund</t>
   </si>
   <si>
-    <t>labor market outcomes a function of network size</t>
-  </si>
-  <si>
     <t>Calvo-Armengol</t>
   </si>
   <si>
@@ -195,9 +177,6 @@
     <t>larger social networks can both help transmit information and heighten competition within the network. Relationship is heterogeneous and dynamic.</t>
   </si>
   <si>
-    <t>Workplace</t>
-  </si>
-  <si>
     <t>Disability program in Norway</t>
   </si>
   <si>
@@ -210,21 +189,12 @@
     <t>Labour market for WW1 vets</t>
   </si>
   <si>
-    <t>"Identification of Endogenous Social Effects: The reflection Problem"</t>
-  </si>
-  <si>
-    <t>"Social Networks and Labor Market Outcomes: Toward and Economic Analysis" AER</t>
-  </si>
-  <si>
     <t>Mortensen and Vishwanath</t>
   </si>
   <si>
     <t>Earnings</t>
   </si>
   <si>
-    <t>"Personal contacts and earnings. It's who you know!"</t>
-  </si>
-  <si>
     <t>Labour Economics</t>
   </si>
   <si>
@@ -243,27 +213,18 @@
     <t>job search in egypt</t>
   </si>
   <si>
-    <t>"Density, Social, Networks, and Job search methods: Theory and application to Egypt"</t>
-  </si>
-  <si>
     <t>Journal of Development Economics</t>
   </si>
   <si>
     <t>Peer effects in education</t>
   </si>
   <si>
-    <t>"Peer Effects, Teacher Incentives, and the Impact of Tracking: Evidence from a Randomized Evaluation in Kenya"</t>
-  </si>
-  <si>
     <t>Durlauf</t>
   </si>
   <si>
     <t>Handbook of Regional and Urban Economics</t>
   </si>
   <si>
-    <t>"Neighborhood Effects"</t>
-  </si>
-  <si>
     <t>Duflo and Saez</t>
   </si>
   <si>
@@ -276,9 +237,6 @@
     <t>Book</t>
   </si>
   <si>
-    <t>"Connections: an introduction to the economics of networks"</t>
-  </si>
-  <si>
     <t>Bandiera and Rasul</t>
   </si>
   <si>
@@ -321,9 +279,6 @@
     <t>Peer effects among teachers</t>
   </si>
   <si>
-    <t>"Teaching Students and Teaching Each Other: The Importance of Peer Learning for Teachers"</t>
-  </si>
-  <si>
     <t>http://works.bepress.com/cgi/viewcontent.cgi?article=1012&amp;context=c_kirabo_jackson</t>
   </si>
   <si>
@@ -438,15 +393,9 @@
     <t>Foster and Rosenzweig</t>
   </si>
   <si>
-    <t>“Learning by Doing and Learning from Others: Human Capital and Technical Change in Agriculture"</t>
-  </si>
-  <si>
     <t>Journal of Political Economy</t>
   </si>
   <si>
-    <t xml:space="preserve"> Ellison and Fudenberg</t>
-  </si>
-  <si>
     <t>The Strength of Weak Ties</t>
   </si>
   <si>
@@ -459,12 +408,6 @@
     <t>Hybrid Corn: An Exploration in the Economics of Technological Change</t>
   </si>
   <si>
-    <t>“Social Learning in a Heterogeneous Population: Technology Diffusion in the Indian Green Revolution</t>
-  </si>
-  <si>
-    <t>“Peer Effects with Random Assignment: Results for Dartmouth Roommates</t>
-  </si>
-  <si>
     <t>Sacerdote, Bruce</t>
   </si>
   <si>
@@ -576,9 +519,6 @@
     <t>http://scholar.harvard.edu/stein/files/thy-neighbor-jf-final.pdf</t>
   </si>
   <si>
-    <t> Calvó-Armengol, Y Zenou</t>
-  </si>
-  <si>
     <t>Job matching, social network and word-of-mouth communication</t>
   </si>
   <si>
@@ -591,9 +531,6 @@
     <t>Online consumer review: Word-of-mouth as a new element of marketing communication mix</t>
   </si>
   <si>
-    <t> Chen, J Xie</t>
-  </si>
-  <si>
     <t>Management Science</t>
   </si>
   <si>
@@ -618,27 +555,15 @@
     <t>http://econ.ucdenver.edu/beckman/Econ%204001/Hirshleifer-cascade-jep.pdf</t>
   </si>
   <si>
-    <t> Is Bigger Better? Customer Base Expansion through Word-of-Mouth Reputation</t>
-  </si>
-  <si>
-    <t> Rob, A Fishman</t>
-  </si>
-  <si>
     <t>http://www.jstor.org/discover/10.1086/444552?uid=3739936&amp;uid=2&amp;uid=4&amp;uid=3739256&amp;sid=21102733807953</t>
   </si>
   <si>
-    <t> Ahn, M Suominen</t>
-  </si>
-  <si>
     <t>Word‐Of‐Mouth Communication and Community Enforcement</t>
   </si>
   <si>
     <t>o</t>
   </si>
   <si>
-    <t> Goolsbee, PJ Klenow</t>
-  </si>
-  <si>
     <t>related</t>
   </si>
   <si>
@@ -663,9 +588,6 @@
     <t>Information cascades: Replication and an extension to majority rule and conformity-rewarding institutions</t>
   </si>
   <si>
-    <t> Hung, CR Plott </t>
-  </si>
-  <si>
     <t>Distinguishing informational cascades from herd behavior in the laboratory</t>
   </si>
   <si>
@@ -732,9 +654,6 @@
     <t>Learning from private and public observations of othersʼ actions</t>
   </si>
   <si>
-    <t> Amador, PO Weill</t>
-  </si>
-  <si>
     <t>http://www.sciencedirect.com/science/article/pii/S0022053112000439</t>
   </si>
   <si>
@@ -874,6 +793,111 @@
   </si>
   <si>
     <t>Sorenson, Alan</t>
+  </si>
+  <si>
+    <t>http://www.hss.caltech.edu/~mshum/gradio/papers/eshin.pdf</t>
+  </si>
+  <si>
+    <t>Banerjee, AG Chandrasekhar, E Duflo, MO Jackson</t>
+  </si>
+  <si>
+    <t>The diffusion of microfinance</t>
+  </si>
+  <si>
+    <t>Who gets the job referral? Evidence from a social networks experiment</t>
+  </si>
+  <si>
+    <t>http://www.aeaweb.org/articles.php?f=s&amp;doi=10.1257/aer.102.7.3574</t>
+  </si>
+  <si>
+    <t>Beaman, J Magruder </t>
+  </si>
+  <si>
+    <t>Social networks and the dynamics of labour market outcomes: evidence from refugees resettled in the US</t>
+  </si>
+  <si>
+    <t>Review of Economics Studies</t>
+  </si>
+  <si>
+    <t>http://restud.oxfordjournals.org/content/79/1/128.short</t>
+  </si>
+  <si>
+    <t>Dahl, AR Kostol, M Mogstad</t>
+  </si>
+  <si>
+    <t>Family Welfare Cultures</t>
+  </si>
+  <si>
+    <t>http://www.econ.brown.edu/econ/events/mogstad.pdf</t>
+  </si>
+  <si>
+    <t>Executive networks and firm policies: Evidence from the random assignment of MBA peers</t>
+  </si>
+  <si>
+    <t>Review of Financial Studies</t>
+  </si>
+  <si>
+    <t>Ahn, M Suominen</t>
+  </si>
+  <si>
+    <t>Amador, PO Weill</t>
+  </si>
+  <si>
+    <t>Calvó-Armengol, Y Zenou</t>
+  </si>
+  <si>
+    <t>Chen, J Xie</t>
+  </si>
+  <si>
+    <t>Goolsbee, PJ Klenow</t>
+  </si>
+  <si>
+    <t>Hung, CR Plott</t>
+  </si>
+  <si>
+    <t>Rob, A Fishman</t>
+  </si>
+  <si>
+    <t>Learning About a New Technology: Pineapple in Ghana</t>
+  </si>
+  <si>
+    <t>Peer Effects, Teacher Incentives, and the Impact of Tracking: Evidence from a Randomized Evaluation in Kenya</t>
+  </si>
+  <si>
+    <t>Neighborhood Effects</t>
+  </si>
+  <si>
+    <t>Learning by Doing and Learning from Others: Human Capital and Technical Change in Agriculture</t>
+  </si>
+  <si>
+    <t>Connections: an introduction to the economics of networks</t>
+  </si>
+  <si>
+    <t>Teaching Students and Teaching Each Other: The Importance of Peer Learning for Teachers</t>
+  </si>
+  <si>
+    <t>Identification of Endogenous Social Effects: The reflection Problem</t>
+  </si>
+  <si>
+    <t>Social Networks and Labor Market Outcomes: Toward and Economic Analysis</t>
+  </si>
+  <si>
+    <t>Personal contacts and earnings. It's who you know!</t>
+  </si>
+  <si>
+    <t>Social Learning in a Heterogeneous Population: Technology Diffusion in the Indian Green Revolution</t>
+  </si>
+  <si>
+    <t>Is Bigger Better? Customer Base Expansion through Word-of-Mouth Reputation</t>
+  </si>
+  <si>
+    <t>Peer Effects with Random Assignment: Results for Dartmouth Roommates</t>
+  </si>
+  <si>
+    <t>Density, Social, Networks, and Job search methods: Theory and application to Egypt</t>
+  </si>
+  <si>
+    <t>Rules of Thumb for Social Learning</t>
   </si>
 </sst>
 </file>
@@ -932,7 +956,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -943,6 +967,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1238,10 +1266,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L108"/>
+  <dimension ref="A1:L105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B79" workbookViewId="0">
-      <selection activeCell="F109" sqref="F109"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1251,7 +1279,7 @@
     <col min="3" max="3" width="12" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.5703125" style="3" customWidth="1"/>
     <col min="5" max="5" width="5.85546875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="93.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="95.7109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="34.140625" style="3" customWidth="1"/>
     <col min="8" max="8" width="255.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="60.42578125" style="2" bestFit="1" customWidth="1"/>
@@ -1261,367 +1289,400 @@
     <col min="13" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:12">
+      <c r="A1" s="3">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="D1" s="3" t="s">
-        <v>142</v>
+        <v>208</v>
       </c>
       <c r="E1" s="7">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="3" t="s">
+        <v>2010</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>205</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="3">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3">
+        <v>186</v>
+      </c>
       <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E2" s="7">
+        <v>2011</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E3" s="7">
+        <v>2001</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="E2" s="7">
-        <v>2001</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="G3" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="D4" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="E4" s="7">
+        <v>2012</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5" s="7">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" s="7">
+        <v>2007</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="7">
+        <v>2006</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="E9" s="7">
+        <v>2012</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="D3" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="E3" s="7">
-        <v>2012</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="3">
+      <c r="I9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="3">
         <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="E4" s="7">
-        <v>2005</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="3">
-        <v>7</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="E5" s="7">
-        <v>2008</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="3">
-        <v>0</v>
-      </c>
-      <c r="B6" s="3">
-        <v>353</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="E6" s="7">
-        <v>2002</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="3">
-        <v>0</v>
-      </c>
-      <c r="B7" s="3">
-        <v>194</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="E7" s="7">
-        <v>2001</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="3">
-        <v>0</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="E8" s="7">
-        <v>2005</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="3">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="E9" s="7">
-        <v>2010</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3">
-        <v>186</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>219</v>
+      <c r="D10" s="6" t="s">
+        <v>199</v>
       </c>
       <c r="E10" s="7">
-        <v>2011</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>217</v>
+        <v>2004</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>154</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="3">
         <v>0</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="E11" s="7">
         <v>2009</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:12">
       <c r="A12" s="3">
         <v>0</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="7">
+        <v>2008</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="E12" s="7">
-        <v>2007</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="3">
-        <v>0</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="E13" s="7">
-        <v>2006</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>249</v>
+        <v>2012</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>265</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>250</v>
+        <v>266</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="3">
-        <v>0</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="D14" s="3" t="s">
-        <v>29</v>
+        <v>264</v>
       </c>
       <c r="E14" s="7">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>2012</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="3">
         <v>0</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>29</v>
+        <v>142</v>
       </c>
       <c r="E15" s="7">
-        <v>2008</v>
+        <v>2000</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>225</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="3">
         <v>0</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E16" s="7">
-        <v>1992</v>
+        <v>1999</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="3">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>225</v>
+      <c r="D17" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="E17" s="7">
-        <v>2004</v>
+        <v>1992</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>172</v>
+        <v>254</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E18" s="7">
-        <v>2012</v>
+        <v>2009</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1629,68 +1690,63 @@
         <v>0</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="E19" s="7">
+        <v>2001</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="C20" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E20" s="7">
         <v>2009</v>
       </c>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="3">
-        <v>0</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="7">
-        <v>2008</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>248</v>
+      <c r="F20" s="6" t="s">
+        <v>219</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="3">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="B21" s="3">
+        <v>229</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>41</v>
+        <v>217</v>
       </c>
       <c r="E21" s="7">
-        <v>2012</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>57</v>
+        <v>2007</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1698,73 +1754,76 @@
         <v>0</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E22" s="7">
-        <v>2000</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>61</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>161</v>
+        <v>235</v>
       </c>
       <c r="E23" s="7">
-        <v>2000</v>
+        <v>2012</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>162</v>
+        <v>236</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>252</v>
+        <v>238</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="3">
-        <v>0</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="D24" s="3" t="s">
-        <v>44</v>
+        <v>250</v>
       </c>
       <c r="E24" s="7">
-        <v>1999</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>42</v>
+        <v>2009</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="3">
-        <v>0</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="D25" s="3" t="s">
-        <v>33</v>
+        <v>233</v>
       </c>
       <c r="E25" s="7">
-        <v>1992</v>
+        <v>2012</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>281</v>
+        <v>234</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>198</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1772,89 +1831,79 @@
         <v>0</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="E26" s="7">
-        <v>2009</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>171</v>
+        <v>2004</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>154</v>
+        <v>161</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>275</v>
       </c>
       <c r="E27" s="7">
-        <v>2001</v>
+        <v>2005</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>89</v>
+        <v>168</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="28" spans="1:12">
+      <c r="A28" s="3">
+        <v>0</v>
+      </c>
       <c r="C28" s="3" t="s">
-        <v>95</v>
+        <v>31</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>245</v>
+        <v>18</v>
       </c>
       <c r="E28" s="7">
-        <v>2009</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="H28" s="1"/>
+        <v>2011</v>
+      </c>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="3">
         <v>0</v>
       </c>
-      <c r="B29" s="3">
-        <v>229</v>
-      </c>
       <c r="C29" s="3" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>244</v>
+        <v>133</v>
       </c>
       <c r="E29" s="7">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>211</v>
+        <v>132</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>212</v>
+        <v>75</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>213</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -1862,325 +1911,367 @@
         <v>0</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="E30" s="7">
-        <v>1975</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>262</v>
+        <v>107</v>
       </c>
       <c r="E31" s="7">
-        <v>2012</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>40</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="32" spans="1:12">
+      <c r="A32" s="3">
+        <v>0</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="D32" s="3" t="s">
-        <v>277</v>
+        <v>108</v>
       </c>
       <c r="E32" s="7">
-        <v>2009</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="3">
+        <v>0</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="D33" s="3" t="s">
-        <v>260</v>
+        <v>110</v>
       </c>
       <c r="E33" s="7">
-        <v>2012</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" s="3">
         <v>0</v>
       </c>
+      <c r="B34" s="3">
+        <v>180</v>
+      </c>
       <c r="C34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>53</v>
+        <v>31</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>198</v>
       </c>
       <c r="E34" s="7">
         <v>2004</v>
       </c>
-      <c r="I34" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
-      <c r="A35" s="3">
-        <v>0</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>19</v>
+      <c r="F34" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="D35" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="E35" s="7">
+        <v>2004</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="3">
+        <v>0</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" s="7">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="3">
+        <v>7</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="E37" s="7">
+        <v>2008</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="D38" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E38" s="7">
         <v>2011</v>
       </c>
-    </row>
-    <row r="36" spans="1:11">
-      <c r="A36" s="3">
-        <v>0</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="E36" s="7">
+      <c r="F38" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="3">
+        <v>9</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E39" s="7">
         <v>2006</v>
       </c>
-      <c r="F36" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="G36" s="3" t="s">
+      <c r="F39" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="3">
+        <v>0</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E40" s="7">
+        <v>2007</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I40" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
-      <c r="A37" s="3">
-        <v>0</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D37" s="3" t="s">
+      <c r="J40" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="3">
+        <v>0</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" s="7">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="C42" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E42" s="7">
+        <v>2010</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="3">
+        <v>0</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="E43" s="7">
+        <v>2013</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="3">
+        <v>0</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E44" s="7">
+        <v>2010</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="3">
+        <v>0</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E45" s="7">
+        <v>2003</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="3">
+        <v>0</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E46" s="7">
+        <v>2011</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="3">
+        <v>0</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E47" s="7">
+        <v>2004</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="C48" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="E48" s="7">
         <v>2010</v>
       </c>
-    </row>
-    <row r="38" spans="1:11">
-      <c r="A38" s="3">
-        <v>0</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E38" s="7">
-        <v>2009</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11">
-      <c r="A39" s="3">
-        <v>0</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E39" s="7">
-        <v>2008</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
-      <c r="A40" s="3">
-        <v>0</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="E40" s="7">
-        <v>1991</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
-      <c r="A41" s="3">
-        <v>0</v>
-      </c>
-      <c r="B41" s="3">
-        <v>180</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="E41" s="7">
-        <v>2004</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11">
-      <c r="D42" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="E42" s="7">
-        <v>2004</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11">
-      <c r="A43" s="3">
-        <v>0</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E43" s="7">
-        <v>2004</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11">
-      <c r="D44" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="E44" s="7">
-        <v>2011</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11">
-      <c r="A45" s="3">
-        <v>9</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="E45" s="7">
-        <v>2006</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11">
-      <c r="A46" s="3">
-        <v>0</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E46" s="7">
-        <v>2007</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="I46" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11">
-      <c r="A47" s="3">
-        <v>0</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E47" s="7">
-        <v>1966</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11">
-      <c r="D48" s="3" t="s">
-        <v>138</v>
+      <c r="F48" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -2188,71 +2279,56 @@
         <v>0</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="E49" s="7">
-        <v>2012</v>
+        <v>2003</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:11">
-      <c r="A50" s="3">
-        <v>0</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="D50" s="3" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="E50" s="7">
-        <v>2010</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>119</v>
+        <v>1993</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>293</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>82</v>
+        <v>229</v>
       </c>
       <c r="E51" s="7">
-        <v>2003</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>279</v>
+        <v>1995</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>156</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="I51" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="J51" s="2" t="s">
-        <v>38</v>
+        <v>225</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -2260,22 +2336,19 @@
         <v>0</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>18</v>
+        <v>145</v>
       </c>
       <c r="E52" s="7">
-        <v>2011</v>
+        <v>2006</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>78</v>
+        <v>144</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="I52" s="2" t="s">
-        <v>77</v>
+        <v>146</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -2283,36 +2356,27 @@
         <v>0</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="E53" s="7">
-        <v>2004</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>80</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="54" spans="1:11">
-      <c r="C54" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="D54" s="3" t="s">
-        <v>282</v>
+        <v>124</v>
       </c>
       <c r="E54" s="7">
-        <v>2010</v>
+        <v>1995</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>283</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>284</v>
+        <v>125</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -2320,39 +2384,42 @@
         <v>0</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>51</v>
+        <v>173</v>
       </c>
       <c r="E55" s="7">
         <v>2003</v>
       </c>
-      <c r="I55" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K55" s="2" t="s">
-        <v>56</v>
+      <c r="F55" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="56" spans="1:11">
       <c r="A56" s="3">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>175</v>
+        <v>137</v>
+      </c>
+      <c r="E56" s="7">
+        <v>1996</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>138</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>176</v>
+        <v>225</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -2360,47 +2427,59 @@
         <v>0</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>164</v>
+        <v>230</v>
       </c>
       <c r="E57" s="7">
-        <v>2006</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>163</v>
+        <v>2010</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>197</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>165</v>
+        <v>201</v>
       </c>
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="3">
         <v>0</v>
       </c>
+      <c r="B58" s="3">
+        <v>353</v>
+      </c>
       <c r="C58" s="3" t="s">
-        <v>5</v>
+        <v>182</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>34</v>
+        <v>277</v>
       </c>
       <c r="E58" s="7">
-        <v>1954</v>
+        <v>2002</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="59" spans="1:11">
+      <c r="C59" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="D59" s="3" t="s">
-        <v>139</v>
+        <v>71</v>
       </c>
       <c r="E59" s="7">
-        <v>1995</v>
+        <v>2012</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>141</v>
+        <v>284</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -2408,42 +2487,33 @@
         <v>0</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>194</v>
+        <v>82</v>
       </c>
       <c r="E60" s="7">
-        <v>2003</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>195</v>
+        <v>2008</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>196</v>
+        <v>226</v>
       </c>
     </row>
     <row r="61" spans="1:11">
-      <c r="A61" s="3">
-        <v>0</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="D61" s="3" t="s">
-        <v>156</v>
+        <v>127</v>
       </c>
       <c r="E61" s="7">
-        <v>1996</v>
+        <v>1973</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>157</v>
+        <v>126</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>252</v>
+        <v>128</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -2451,67 +2521,76 @@
         <v>0</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>257</v>
+        <v>122</v>
       </c>
       <c r="E62" s="7">
-        <v>2010</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>227</v>
+        <v>1957</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="63" spans="1:11">
+      <c r="A63" s="3">
+        <v>0</v>
+      </c>
       <c r="C63" s="3" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="E63" s="7">
-        <v>2012</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>86</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="64" spans="1:11">
       <c r="A64" s="3">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>96</v>
+        <v>161</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>163</v>
       </c>
       <c r="E64" s="7">
-        <v>2008</v>
-      </c>
-      <c r="F64" s="3" t="s">
-        <v>97</v>
+        <v>2005</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>164</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>253</v>
+        <v>165</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="65" spans="1:10">
+      <c r="A65" s="3">
+        <v>0</v>
+      </c>
+      <c r="B65" s="3">
+        <v>194</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="D65" s="3" t="s">
-        <v>144</v>
+        <v>278</v>
       </c>
       <c r="E65" s="7">
-        <v>1973</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>143</v>
+        <v>2001</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>189</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>145</v>
+        <v>224</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -2519,16 +2598,16 @@
         <v>0</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>137</v>
+        <v>40</v>
       </c>
       <c r="E66" s="7">
-        <v>1957</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>146</v>
+        <v>2004</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -2536,13 +2615,28 @@
         <v>0</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>200</v>
       </c>
       <c r="E67" s="7">
-        <v>2008</v>
+        <v>2007</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -2550,36 +2644,51 @@
         <v>0</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="E68" s="7">
         <v>2009</v>
       </c>
+      <c r="F68" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="J68" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="3">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>182</v>
+        <v>10</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="E69" s="7">
-        <v>2005</v>
+        <v>2010</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>183</v>
+        <v>117</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>184</v>
+        <v>116</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>185</v>
+        <v>115</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -2590,13 +2699,10 @@
         <v>7</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="E70" s="7">
-        <v>2004</v>
-      </c>
-      <c r="I70" s="2" t="s">
-        <v>62</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -2604,28 +2710,28 @@
         <v>0</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>226</v>
+        <v>31</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="E71" s="7">
-        <v>2007</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>108</v>
+        <v>2009</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>285</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>254</v>
+        <v>85</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="J71" s="2" t="s">
-        <v>111</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -2633,51 +2739,27 @@
         <v>0</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>117</v>
+        <v>14</v>
       </c>
       <c r="E72" s="7">
-        <v>2009</v>
-      </c>
-      <c r="F72" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="G72" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I72" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="J72" s="2" t="s">
-        <v>43</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="73" spans="1:10">
-      <c r="A73" s="3">
-        <v>0</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="D73" s="3" t="s">
-        <v>11</v>
+        <v>243</v>
       </c>
       <c r="E73" s="7">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>132</v>
+        <v>245</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="H73" s="1" t="s">
-        <v>130</v>
+        <v>244</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -2685,13 +2767,13 @@
         <v>0</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E74" s="7">
-        <v>2010</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -2699,28 +2781,28 @@
         <v>0</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="E75" s="7">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>99</v>
+        <v>226</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -2728,41 +2810,47 @@
         <v>0</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>14</v>
+        <v>140</v>
       </c>
       <c r="E76" s="7">
-        <v>1955</v>
+        <v>2008</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="77" spans="1:10">
+      <c r="A77" s="3">
+        <v>0</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="D77" s="3" t="s">
-        <v>270</v>
+        <v>23</v>
       </c>
       <c r="E77" s="7">
-        <v>2012</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="G77" s="3" t="s">
-        <v>271</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="78" spans="1:10">
-      <c r="A78" s="3">
-        <v>0</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="D78" s="3" t="s">
-        <v>22</v>
+        <v>214</v>
       </c>
       <c r="E78" s="7">
-        <v>2007</v>
+        <v>2009</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -2770,28 +2858,16 @@
         <v>0</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>95</v>
+        <v>31</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>91</v>
+        <v>44</v>
       </c>
       <c r="E79" s="7">
-        <v>2007</v>
-      </c>
-      <c r="F79" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="G79" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="H79" s="1" t="s">
-        <v>93</v>
+        <v>2009</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="J79" s="2" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -2799,19 +2875,13 @@
         <v>0</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>159</v>
+        <v>13</v>
       </c>
       <c r="E80" s="7">
-        <v>2008</v>
-      </c>
-      <c r="F80" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="G80" s="3" t="s">
-        <v>160</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -2819,27 +2889,42 @@
         <v>0</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>26</v>
+        <v>113</v>
       </c>
       <c r="E81" s="7">
-        <v>2011</v>
+        <v>2007</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="J81" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="82" spans="1:10">
+      <c r="A82" s="3">
+        <v>0</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="D82" s="3" t="s">
-        <v>241</v>
+        <v>25</v>
       </c>
       <c r="E82" s="7">
-        <v>2009</v>
+        <v>1993</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="G82" s="3" t="s">
-        <v>171</v>
+        <v>286</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -2847,30 +2932,42 @@
         <v>0</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="E83" s="7">
         <v>2009</v>
       </c>
-      <c r="I83" s="2" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="84" spans="1:10">
       <c r="A84" s="3">
         <v>0</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>13</v>
+        <v>119</v>
       </c>
       <c r="E84" s="7">
-        <v>1944</v>
+        <v>2003</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="I84" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J84" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -2878,42 +2975,36 @@
         <v>0</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>128</v>
+        <v>45</v>
       </c>
       <c r="E85" s="7">
-        <v>2007</v>
-      </c>
-      <c r="F85" s="6" t="s">
-        <v>127</v>
+        <v>2001</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>287</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="H85" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="J85" s="2" t="s">
-        <v>43</v>
+        <v>224</v>
+      </c>
+      <c r="I85" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="86" spans="1:10">
-      <c r="A86" s="3">
-        <v>0</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="D86" s="3" t="s">
-        <v>30</v>
+        <v>248</v>
       </c>
       <c r="E86" s="7">
-        <v>1993</v>
+        <v>2011</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>64</v>
+        <v>249</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -2921,13 +3012,22 @@
         <v>0</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="E87" s="7">
-        <v>2009</v>
+        <v>1994</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -2935,28 +3035,19 @@
         <v>0</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>134</v>
+        <v>42</v>
       </c>
       <c r="E88" s="7">
         <v>2003</v>
       </c>
-      <c r="F88" s="3" t="s">
-        <v>133</v>
-      </c>
       <c r="G88" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H88" s="2" t="s">
-        <v>135</v>
+        <v>225</v>
       </c>
       <c r="I88" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="J88" s="2" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -2964,33 +3055,42 @@
         <v>0</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E89" s="7">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="F89" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="G89" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I89" s="2" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="90" spans="1:10">
+      <c r="A90" s="3">
+        <v>0</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="D90" s="3" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="E90" s="7">
-        <v>2011</v>
-      </c>
-      <c r="F90" s="3" t="s">
-        <v>276</v>
+        <v>2005</v>
+      </c>
+      <c r="F90" s="6" t="s">
+        <v>290</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>72</v>
+        <v>125</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -2998,22 +3098,19 @@
         <v>0</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>66</v>
+        <v>149</v>
       </c>
       <c r="E91" s="7">
-        <v>1994</v>
+        <v>2001</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>68</v>
+        <v>147</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="I91" s="2" t="s">
-        <v>67</v>
+        <v>148</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -3021,62 +3118,53 @@
         <v>0</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="E92" s="7">
         <v>2003</v>
       </c>
-      <c r="F92" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G92" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="I92" s="2" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="93" spans="1:10">
       <c r="A93" s="3">
         <v>0</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="E93" s="7">
-        <v>2002</v>
-      </c>
-      <c r="F93" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="G93" s="3" t="s">
-        <v>76</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="94" spans="1:10">
       <c r="A94" s="3">
         <v>0</v>
       </c>
+      <c r="B94" s="3">
+        <v>1216</v>
+      </c>
       <c r="C94" s="3" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>168</v>
+        <v>231</v>
       </c>
       <c r="E94" s="7">
-        <v>2001</v>
-      </c>
-      <c r="F94" s="3" t="s">
-        <v>166</v>
+        <v>1998</v>
+      </c>
+      <c r="F94" s="6" t="s">
+        <v>176</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>167</v>
+        <v>177</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -3084,13 +3172,13 @@
         <v>0</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E95" s="7">
-        <v>2003</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -3098,53 +3186,56 @@
         <v>0</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>12</v>
+        <v>130</v>
       </c>
       <c r="E96" s="7">
-        <v>1943</v>
+        <v>2001</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="97" spans="1:9">
       <c r="A97" s="3">
         <v>0</v>
       </c>
-      <c r="B97" s="3">
-        <v>1216</v>
-      </c>
       <c r="C97" s="3" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>258</v>
+        <v>19</v>
       </c>
       <c r="E97" s="7">
-        <v>1998</v>
-      </c>
-      <c r="F97" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="G97" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="H97" s="1" t="s">
-        <v>199</v>
+        <v>2013</v>
+      </c>
+      <c r="F97" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="G97" s="9" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="98" spans="1:9">
-      <c r="A98" s="3">
-        <v>0</v>
-      </c>
       <c r="C98" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D98" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>210</v>
       </c>
       <c r="E98" s="7">
-        <v>2001</v>
+        <v>2000</v>
+      </c>
+      <c r="F98" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -3152,260 +3243,217 @@
         <v>0</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D99" s="3" t="s">
-        <v>149</v>
+        <v>31</v>
+      </c>
+      <c r="D99" s="6" t="s">
+        <v>195</v>
       </c>
       <c r="E99" s="7">
+        <v>2006</v>
+      </c>
+      <c r="F99" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
+      <c r="D100" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E100" s="7">
+        <v>2006</v>
+      </c>
+      <c r="F100" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
+      <c r="A101" s="3">
+        <v>0</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E101" s="7">
         <v>2001</v>
       </c>
-      <c r="F99" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="G99" s="3" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9">
-      <c r="A100" s="3">
-        <v>0</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D100" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E100" s="7">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9">
-      <c r="C101" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D101" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="E101" s="7">
-        <v>2000</v>
-      </c>
-      <c r="F101" s="6" t="s">
-        <v>235</v>
+      <c r="F101" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>212</v>
+        <v>62</v>
+      </c>
+      <c r="I101" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="102" spans="1:9">
-      <c r="A102" s="3">
-        <v>0</v>
-      </c>
       <c r="C102" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D102" s="6" t="s">
-        <v>221</v>
+        <v>239</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>240</v>
       </c>
       <c r="E102" s="7">
-        <v>2006</v>
-      </c>
-      <c r="F102" s="6" t="s">
-        <v>220</v>
+        <v>2013</v>
+      </c>
+      <c r="F102" s="3" t="s">
+        <v>241</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>222</v>
+        <v>242</v>
       </c>
     </row>
     <row r="103" spans="1:9">
+      <c r="A103" s="3">
+        <v>0</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="D103" s="3" t="s">
-        <v>285</v>
+        <v>63</v>
       </c>
       <c r="E103" s="7">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>280</v>
+        <v>292</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>269</v>
+        <v>65</v>
+      </c>
+      <c r="I103" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="104" spans="1:9">
       <c r="A104" s="3">
         <v>0</v>
       </c>
+      <c r="B104" s="3">
+        <v>156</v>
+      </c>
       <c r="C104" s="3" t="s">
-        <v>36</v>
+        <v>182</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>46</v>
+        <v>203</v>
       </c>
       <c r="E104" s="7">
-        <v>2001</v>
-      </c>
-      <c r="F104" s="3" t="s">
-        <v>71</v>
+        <v>2009</v>
+      </c>
+      <c r="F104" s="6" t="s">
+        <v>202</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="I104" s="2" t="s">
-        <v>42</v>
+        <v>224</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="105" spans="1:9">
+      <c r="A105" s="3">
+        <v>0</v>
+      </c>
       <c r="C105" s="3" t="s">
-        <v>266</v>
+        <v>31</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>267</v>
+        <v>151</v>
       </c>
       <c r="E105" s="7">
-        <v>2013</v>
+        <v>2003</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>268</v>
+        <v>150</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9">
-      <c r="A106" s="3">
-        <v>0</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D106" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E106" s="7">
-        <v>2005</v>
-      </c>
-      <c r="F106" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G106" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="I106" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9">
-      <c r="A107" s="3">
-        <v>0</v>
-      </c>
-      <c r="B107" s="3">
-        <v>156</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="E107" s="7">
-        <v>2009</v>
-      </c>
-      <c r="F107" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="G107" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="H107" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9">
-      <c r="A108" s="3">
-        <v>0</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="E108" s="7">
-        <v>2003</v>
-      </c>
-      <c r="F108" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="G108" s="3" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:L108">
-    <sortCondition ref="D107"/>
+  <sortState ref="A1:L105">
+    <sortCondition ref="D4"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="H79" r:id="rId1"/>
-    <hyperlink ref="H75" r:id="rId2"/>
-    <hyperlink ref="F26" r:id="rId3" display="http://www.mitpressjournals.org/doi/abs/10.1162/rest.91.4.695"/>
-    <hyperlink ref="F71" r:id="rId4" display="http://rfs.oxfordjournals.org/content/20/4/1327.short"/>
-    <hyperlink ref="H71" r:id="rId5"/>
-    <hyperlink ref="F12" r:id="rId6" display="http://onlinelibrary.wiley.com/doi/10.1002/jae.924/full"/>
-    <hyperlink ref="D12" r:id="rId7" display="http://scholar.google.com/citations?user=AEdHwUoAAAAJ&amp;hl=en&amp;oi=sra"/>
-    <hyperlink ref="F72" r:id="rId8" display="http://www.aeaweb.org/articles.php?doi=10.1257/app.1.4.34"/>
-    <hyperlink ref="H72" r:id="rId9"/>
-    <hyperlink ref="F50" r:id="rId10" display="http://www.jstor.org/stable/10.2307/25760213"/>
-    <hyperlink ref="F85" r:id="rId11" display="http://www.mitpressjournals.org/doi/abs/10.1162/rest.89.2.289"/>
-    <hyperlink ref="H85" r:id="rId12"/>
-    <hyperlink ref="H73" r:id="rId13"/>
-    <hyperlink ref="F73" r:id="rId14" display="http://www.stanford.edu/~jacksonm/socialnetecon-chapter.pdf"/>
-    <hyperlink ref="H36" r:id="rId15"/>
-    <hyperlink ref="F36" r:id="rId16" display="http://www.rwj.harvard.edu/scholarsmaterials/carman/SocialInfluences.pdf"/>
-    <hyperlink ref="D17" r:id="rId17" display="http://scholar.google.com/citations?user=XCo4OfoAAAAJ&amp;hl=en&amp;oi=sra"/>
-    <hyperlink ref="F56" r:id="rId18" display="http://qje.oxfordjournals.org/content/110/1/93.short"/>
-    <hyperlink ref="H56" r:id="rId19"/>
-    <hyperlink ref="F45" r:id="rId20" display="http://www.jstor.org/stable/10.2307/30162409"/>
-    <hyperlink ref="D69" r:id="rId21" display="http://scholar.google.com/citations?user=ctHVoM8AAAAJ&amp;hl=en&amp;oi=sra"/>
-    <hyperlink ref="F69" r:id="rId22" display="http://onlinelibrary.wiley.com/doi/10.1111/j.1540-6261.2005.00817.x/full"/>
-    <hyperlink ref="H69" r:id="rId23"/>
-    <hyperlink ref="D4" r:id="rId24" display="http://scholar.google.com/citations?user=Yh5OxAcAAAAJ&amp;hl=en&amp;oi=sra"/>
-    <hyperlink ref="F4" r:id="rId25" display="http://www.sciencedirect.com/science/article/pii/S0094119005000021"/>
-    <hyperlink ref="F5" r:id="rId26" display="http://mansci.journal.informs.org/content/54/3/477.short"/>
-    <hyperlink ref="H5" r:id="rId27" display="http://student.bus.olemiss.edu/files/conlon/others/Others/Camera/Online buyers' preferences/Chen et al 2008.pdf"/>
-    <hyperlink ref="F60" r:id="rId28" display="http://www.sciencedirect.com/science/article/pii/S0899825603001441"/>
-    <hyperlink ref="H60" r:id="rId29"/>
-    <hyperlink ref="F97" r:id="rId30" display="http://www.jstor.org/stable/10.2307/2647037"/>
-    <hyperlink ref="H97" r:id="rId31" display="http://econ.ucdenver.edu/beckman/Econ 4001/Hirshleifer-cascade-jep.pdf"/>
-    <hyperlink ref="F8" r:id="rId32" display="http://ideas.repec.org/a/ucp/jpolec/v113y2005i5p1146-1175.html"/>
-    <hyperlink ref="H8" r:id="rId33"/>
-    <hyperlink ref="D2" r:id="rId34" display="http://scholar.google.com/citations?user=jpuCxCUAAAAJ&amp;hl=en&amp;oi=sra"/>
-    <hyperlink ref="F2" r:id="rId35" display="http://onlinelibrary.wiley.com/doi/10.1111/1468-2354.00115/full"/>
-    <hyperlink ref="H6" r:id="rId36" display="https://26c27f06-a-62cb3a1a-s-sites.googlegroups.com/site/organizacionindustrialunmsm/classroom-news/listadelecturasparalasexposiciones/GoolsbeeandKlenow%282002%29.pdf?attachauth=ANoY7cplyfy94UZDYvreLOj1K29MdMqnshgnD4p3gI0yI7viXIU_Rn_o_1E5tuuqquMew4CP-wwxDZ0-8QEqCVdLN3Pwvo58-7J6jx8v5N8Wt_CSJ25HUI32piQAUJsacLqWq5qjfDRrLNamszxf7X69x0wTdsIpghPNbEe-DwK1kYm2WaIps5rwaHJHDRgi9Hv1WzE-IoNghT6wqoEx8LQAsNxahN94joXUtAUf8D5zTiTLm4QxXZIfj2cugEM9agqcNL2X5_x4pp6Pg6p2pE2RiWRp9-S3iGGVRiQbhAWQ6NdaZc7Vc-JYkSVt4W9f5cxpcBAmNtW8&amp;attredirects=0"/>
-    <hyperlink ref="F29" r:id="rId37" display="http://www.sciencedirect.com/science/article/pii/S0022053106001220"/>
-    <hyperlink ref="H29" r:id="rId38"/>
-    <hyperlink ref="F7" r:id="rId39" display="http://www.jstor.org/stable/10.2307/2677936"/>
-    <hyperlink ref="F41" r:id="rId40" display="http://www.jstor.org/stable/10.2307/3592939"/>
-    <hyperlink ref="D41" r:id="rId41" display="http://scholar.google.com/citations?user=438fDpcAAAAJ&amp;hl=en&amp;oi=sra"/>
-    <hyperlink ref="F10" r:id="rId42" display="http://restud.oxfordjournals.org/content/78/4/1201.short"/>
-    <hyperlink ref="H10" r:id="rId43"/>
-    <hyperlink ref="F102" r:id="rId44" display="http://onlinelibrary.wiley.com/doi/10.1111/j.0950-0804.2006.00280.x/full"/>
-    <hyperlink ref="D102" r:id="rId45" display="http://scholar.google.com/citations?user=AEdHwUoAAAAJ&amp;hl=en&amp;oi=sra"/>
-    <hyperlink ref="F62" r:id="rId46" display="http://www.ingentaconnect.com/content/aea/aejmi/2010/00000002/00000001/art00007"/>
-    <hyperlink ref="F107" r:id="rId47" display="http://www.ingentaconnect.com/content/aea/aer/2009/00000099/00000005/art00009"/>
-    <hyperlink ref="H107" r:id="rId48"/>
-    <hyperlink ref="F9" r:id="rId49" display="http://www.sciencedirect.com/science/article/pii/S0899825610000217"/>
-    <hyperlink ref="F42" r:id="rId50" display="http://www.sciencedirect.com/science/article/pii/S0899825603001799"/>
-    <hyperlink ref="D42" r:id="rId51" display="http://scholar.google.com/citations?user=438fDpcAAAAJ&amp;hl=en&amp;oi=sra"/>
-    <hyperlink ref="F101" r:id="rId52" display="http://www.sciencedirect.com/science/article/pii/S0022053100927017"/>
-    <hyperlink ref="F3" r:id="rId53" display="http://www.sciencedirect.com/science/article/pii/S0022053112000439"/>
-    <hyperlink ref="D3" r:id="rId54" display="http://scholar.google.com/citations?user=M695hyAAAAAJ&amp;hl=en&amp;oi=sra"/>
-    <hyperlink ref="H3" r:id="rId55"/>
-    <hyperlink ref="H31" r:id="rId56"/>
-    <hyperlink ref="F77" r:id="rId57" display="http://papers.ssrn.com/sol3/papers.cfm?abstract_id=1359006"/>
+    <hyperlink ref="H75" r:id="rId1"/>
+    <hyperlink ref="H71" r:id="rId2"/>
+    <hyperlink ref="F18" r:id="rId3" display="http://www.mitpressjournals.org/doi/abs/10.1162/rest.91.4.695"/>
+    <hyperlink ref="F67" r:id="rId4" display="http://rfs.oxfordjournals.org/content/20/4/1327.short"/>
+    <hyperlink ref="H67" r:id="rId5"/>
+    <hyperlink ref="F6" r:id="rId6" display="http://onlinelibrary.wiley.com/doi/10.1002/jae.924/full"/>
+    <hyperlink ref="D6" r:id="rId7" display="http://scholar.google.com/citations?user=AEdHwUoAAAAJ&amp;hl=en&amp;oi=sra"/>
+    <hyperlink ref="F68" r:id="rId8" display="http://www.aeaweb.org/articles.php?doi=10.1257/app.1.4.34"/>
+    <hyperlink ref="H68" r:id="rId9"/>
+    <hyperlink ref="F44" r:id="rId10" display="http://www.jstor.org/stable/10.2307/25760213"/>
+    <hyperlink ref="F81" r:id="rId11" display="http://www.mitpressjournals.org/doi/abs/10.1162/rest.89.2.289"/>
+    <hyperlink ref="H81" r:id="rId12"/>
+    <hyperlink ref="H69" r:id="rId13"/>
+    <hyperlink ref="F69" r:id="rId14" display="http://www.stanford.edu/~jacksonm/socialnetecon-chapter.pdf"/>
+    <hyperlink ref="H29" r:id="rId15"/>
+    <hyperlink ref="F29" r:id="rId16" display="http://www.rwj.harvard.edu/scholarsmaterials/carman/SocialInfluences.pdf"/>
+    <hyperlink ref="D10" r:id="rId17" display="http://scholar.google.com/citations?user=XCo4OfoAAAAJ&amp;hl=en&amp;oi=sra"/>
+    <hyperlink ref="F51" r:id="rId18" display="http://qje.oxfordjournals.org/content/110/1/93.short"/>
+    <hyperlink ref="H51" r:id="rId19"/>
+    <hyperlink ref="F39" r:id="rId20" display="http://www.jstor.org/stable/10.2307/30162409"/>
+    <hyperlink ref="D64" r:id="rId21" display="http://scholar.google.com/citations?user=ctHVoM8AAAAJ&amp;hl=en&amp;oi=sra"/>
+    <hyperlink ref="F64" r:id="rId22" display="http://onlinelibrary.wiley.com/doi/10.1111/j.1540-6261.2005.00817.x/full"/>
+    <hyperlink ref="H64" r:id="rId23"/>
+    <hyperlink ref="D27" r:id="rId24" display="http://scholar.google.com/citations?user=Yh5OxAcAAAAJ&amp;hl=en&amp;oi=sra"/>
+    <hyperlink ref="F27" r:id="rId25" display="http://www.sciencedirect.com/science/article/pii/S0094119005000021"/>
+    <hyperlink ref="F37" r:id="rId26" display="http://mansci.journal.informs.org/content/54/3/477.short"/>
+    <hyperlink ref="H37" r:id="rId27" display="http://student.bus.olemiss.edu/files/conlon/others/Others/Camera/Online buyers' preferences/Chen et al 2008.pdf"/>
+    <hyperlink ref="F55" r:id="rId28" display="http://www.sciencedirect.com/science/article/pii/S0899825603001441"/>
+    <hyperlink ref="H55" r:id="rId29"/>
+    <hyperlink ref="F94" r:id="rId30" display="http://www.jstor.org/stable/10.2307/2647037"/>
+    <hyperlink ref="H94" r:id="rId31" display="http://econ.ucdenver.edu/beckman/Econ 4001/Hirshleifer-cascade-jep.pdf"/>
+    <hyperlink ref="F90" r:id="rId32" display="http://ideas.repec.org/a/ucp/jpolec/v113y2005i5p1146-1175.html"/>
+    <hyperlink ref="H90" r:id="rId33"/>
+    <hyperlink ref="D3" r:id="rId34" display="http://scholar.google.com/citations?user=jpuCxCUAAAAJ&amp;hl=en&amp;oi=sra"/>
+    <hyperlink ref="F3" r:id="rId35" display="http://onlinelibrary.wiley.com/doi/10.1111/1468-2354.00115/full"/>
+    <hyperlink ref="H58" r:id="rId36" display="https://26c27f06-a-62cb3a1a-s-sites.googlegroups.com/site/organizacionindustrialunmsm/classroom-news/listadelecturasparalasexposiciones/GoolsbeeandKlenow%282002%29.pdf?attachauth=ANoY7cplyfy94UZDYvreLOj1K29MdMqnshgnD4p3gI0yI7viXIU_Rn_o_1E5tuuqquMew4CP-wwxDZ0-8QEqCVdLN3Pwvo58-7J6jx8v5N8Wt_CSJ25HUI32piQAUJsacLqWq5qjfDRrLNamszxf7X69x0wTdsIpghPNbEe-DwK1kYm2WaIps5rwaHJHDRgi9Hv1WzE-IoNghT6wqoEx8LQAsNxahN94joXUtAUf8D5zTiTLm4QxXZIfj2cugEM9agqcNL2X5_x4pp6Pg6p2pE2RiWRp9-S3iGGVRiQbhAWQ6NdaZc7Vc-JYkSVt4W9f5cxpcBAmNtW8&amp;attredirects=0"/>
+    <hyperlink ref="F21" r:id="rId37" display="http://www.sciencedirect.com/science/article/pii/S0022053106001220"/>
+    <hyperlink ref="H21" r:id="rId38"/>
+    <hyperlink ref="F65" r:id="rId39" display="http://www.jstor.org/stable/10.2307/2677936"/>
+    <hyperlink ref="F34" r:id="rId40" display="http://www.jstor.org/stable/10.2307/3592939"/>
+    <hyperlink ref="D34" r:id="rId41" display="http://scholar.google.com/citations?user=438fDpcAAAAJ&amp;hl=en&amp;oi=sra"/>
+    <hyperlink ref="F2" r:id="rId42" display="http://restud.oxfordjournals.org/content/78/4/1201.short"/>
+    <hyperlink ref="H2" r:id="rId43"/>
+    <hyperlink ref="F99" r:id="rId44" display="http://onlinelibrary.wiley.com/doi/10.1111/j.0950-0804.2006.00280.x/full"/>
+    <hyperlink ref="D99" r:id="rId45" display="http://scholar.google.com/citations?user=AEdHwUoAAAAJ&amp;hl=en&amp;oi=sra"/>
+    <hyperlink ref="F57" r:id="rId46" display="http://www.ingentaconnect.com/content/aea/aejmi/2010/00000002/00000001/art00007"/>
+    <hyperlink ref="F104" r:id="rId47" display="http://www.ingentaconnect.com/content/aea/aer/2009/00000099/00000005/art00009"/>
+    <hyperlink ref="H104" r:id="rId48"/>
+    <hyperlink ref="F1" r:id="rId49" display="http://www.sciencedirect.com/science/article/pii/S0899825610000217"/>
+    <hyperlink ref="F35" r:id="rId50" display="http://www.sciencedirect.com/science/article/pii/S0899825603001799"/>
+    <hyperlink ref="D35" r:id="rId51" display="http://scholar.google.com/citations?user=438fDpcAAAAJ&amp;hl=en&amp;oi=sra"/>
+    <hyperlink ref="F98" r:id="rId52" display="http://www.sciencedirect.com/science/article/pii/S0022053100927017"/>
+    <hyperlink ref="F4" r:id="rId53" display="http://www.sciencedirect.com/science/article/pii/S0022053112000439"/>
+    <hyperlink ref="D4" r:id="rId54" display="http://scholar.google.com/citations?user=M695hyAAAAAJ&amp;hl=en&amp;oi=sra"/>
+    <hyperlink ref="H4" r:id="rId55"/>
+    <hyperlink ref="H23" r:id="rId56"/>
+    <hyperlink ref="F73" r:id="rId57" display="http://papers.ssrn.com/sol3/papers.cfm?abstract_id=1359006"/>
+    <hyperlink ref="H9" r:id="rId58"/>
+    <hyperlink ref="F9" r:id="rId59" display="http://www.nber.org/papers/w17743"/>
+    <hyperlink ref="F14" r:id="rId60" display="http://www.ingentaconnect.com/content/aea/aer/2012/00000102/00000007/art00018"/>
+    <hyperlink ref="H14" r:id="rId61"/>
+    <hyperlink ref="F13" r:id="rId62" display="http://restud.oxfordjournals.org/content/79/1/128.short"/>
+    <hyperlink ref="H13" r:id="rId63"/>
+    <hyperlink ref="D43" r:id="rId64" display="http://scholar.google.com/citations?user=nKursZ8AAAAJ&amp;hl=en&amp;oi=sra"/>
+    <hyperlink ref="F97" r:id="rId65" display="http://rfs.oxfordjournals.org/content/26/6/1401.short"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId58"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId66"/>
 </worksheet>
 </file>
 

</xml_diff>